<commit_message>
Minor bug fix. RetirementCorpus, PF Maturity events added
</commit_message>
<xml_diff>
--- a/Excellent.xlsx
+++ b/Excellent.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Project - Learning\Project - Financials\Project - Excellent\Excellent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C5470F2-CABA-4BBB-88B4-6E730E27E6BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{950F6A50-64B7-4482-80E9-D398526914BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="862" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="862" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="1" r:id="rId1"/>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="88">
   <si>
     <t>Name</t>
   </si>
@@ -370,6 +370,9 @@
   </si>
   <si>
     <t>NET INVESTMENT</t>
+  </si>
+  <si>
+    <t>Retirement Corpus</t>
   </si>
 </sst>
 </file>
@@ -482,7 +485,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -635,12 +638,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -828,23 +846,35 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -991,7 +1021,7 @@
             </a:ln>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="27432" bIns="27432" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="ctr" rtl="0">
@@ -1302,8 +1332,8 @@
   </sheetPr>
   <dimension ref="A1:L109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="91" workbookViewId="0">
-      <selection activeCell="H118" sqref="H118"/>
+    <sheetView zoomScale="91" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="41.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1313,7 +1343,7 @@
     <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.85546875" customWidth="1"/>
-    <col min="7" max="7" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="46.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
@@ -1777,23 +1807,23 @@
       </c>
       <c r="F19" s="4">
         <f ca="1">-SUMIFS('Input-Events'!F$4:F$106, 'Input-Events'!E$4:E$106, $C19)</f>
-        <v>0</v>
+        <v>300000</v>
       </c>
       <c r="G19" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G19" ca="1">_xlfn.TEXTJOIN(", ", TRUE, IF('Input-Events'!E$4:E$106=$C19, 'Input-Events'!D$4:D$106, ""))</f>
-        <v/>
+        <v>PPF Maturity, Insurance Maturity</v>
       </c>
       <c r="H19" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>4280096</v>
+        <v>4580096</v>
       </c>
       <c r="I19" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>171204</v>
+        <v>183204</v>
       </c>
       <c r="J19" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>4451300</v>
+        <v>4763300</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
@@ -1807,7 +1837,7 @@
       </c>
       <c r="D20" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>4451300</v>
+        <v>4763300</v>
       </c>
       <c r="E20" s="14">
         <f t="shared" ca="1" si="5"/>
@@ -1823,15 +1853,15 @@
       </c>
       <c r="H20" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>5067022</v>
+        <v>5379022</v>
       </c>
       <c r="I20" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>202681</v>
+        <v>215161</v>
       </c>
       <c r="J20" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>5269703</v>
+        <v>5594183</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
@@ -1845,7 +1875,7 @@
       </c>
       <c r="D21" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>5269703</v>
+        <v>5594183</v>
       </c>
       <c r="E21" s="14">
         <f t="shared" ca="1" si="5"/>
@@ -1861,15 +1891,15 @@
       </c>
       <c r="H21" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>5916211</v>
+        <v>6240691</v>
       </c>
       <c r="I21" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>236648</v>
+        <v>249628</v>
       </c>
       <c r="J21" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>6152859</v>
+        <v>6490319</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
@@ -1883,7 +1913,7 @@
       </c>
       <c r="D22" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>6152859</v>
+        <v>6490319</v>
       </c>
       <c r="E22" s="14">
         <f t="shared" ca="1" si="5"/>
@@ -1899,15 +1929,15 @@
       </c>
       <c r="H22" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>6831692</v>
+        <v>7169152</v>
       </c>
       <c r="I22" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>273268</v>
+        <v>286766</v>
       </c>
       <c r="J22" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>7104960</v>
+        <v>7455918</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
@@ -1921,7 +1951,7 @@
       </c>
       <c r="D23" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>7104960</v>
+        <v>7455918</v>
       </c>
       <c r="E23" s="14">
         <f t="shared" ca="1" si="5"/>
@@ -1937,15 +1967,15 @@
       </c>
       <c r="H23" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>7817735</v>
+        <v>8168693</v>
       </c>
       <c r="I23" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>312709</v>
+        <v>326748</v>
       </c>
       <c r="J23" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>8130444</v>
+        <v>8495441</v>
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
@@ -1959,7 +1989,7 @@
       </c>
       <c r="D24" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>8130444</v>
+        <v>8495441</v>
       </c>
       <c r="E24" s="14">
         <f t="shared" ca="1" si="5"/>
@@ -1975,15 +2005,15 @@
       </c>
       <c r="H24" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>3878858</v>
+        <v>4243855</v>
       </c>
       <c r="I24" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>155154</v>
+        <v>169754</v>
       </c>
       <c r="J24" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>4034012</v>
+        <v>4413609</v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
@@ -1997,7 +2027,7 @@
       </c>
       <c r="D25" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>4034012</v>
+        <v>4413609</v>
       </c>
       <c r="E25" s="14">
         <f t="shared" ca="1" si="5"/>
@@ -2013,15 +2043,15 @@
       </c>
       <c r="H25" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>4819847</v>
+        <v>5199444</v>
       </c>
       <c r="I25" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>192794</v>
+        <v>207978</v>
       </c>
       <c r="J25" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>5012641</v>
+        <v>5407422</v>
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
@@ -2035,7 +2065,7 @@
       </c>
       <c r="D26" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>5012641</v>
+        <v>5407422</v>
       </c>
       <c r="E26" s="14">
         <f t="shared" ca="1" si="5"/>
@@ -2051,15 +2081,15 @@
       </c>
       <c r="H26" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>5837768</v>
+        <v>6232549</v>
       </c>
       <c r="I26" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>233511</v>
+        <v>249302</v>
       </c>
       <c r="J26" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>6071279</v>
+        <v>6481851</v>
       </c>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
@@ -2073,7 +2103,7 @@
       </c>
       <c r="D27" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>6071279</v>
+        <v>6481851</v>
       </c>
       <c r="E27" s="14">
         <f t="shared" ca="1" si="5"/>
@@ -2089,15 +2119,15 @@
       </c>
       <c r="H27" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>6937662</v>
+        <v>7348234</v>
       </c>
       <c r="I27" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>277506</v>
+        <v>293929</v>
       </c>
       <c r="J27" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>7215168</v>
+        <v>7642163</v>
       </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
@@ -2111,7 +2141,7 @@
       </c>
       <c r="D28" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>7215168</v>
+        <v>7642163</v>
       </c>
       <c r="E28" s="14">
         <f t="shared" ca="1" si="5"/>
@@ -2127,15 +2157,15 @@
       </c>
       <c r="H28" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>8124870</v>
+        <v>8551865</v>
       </c>
       <c r="I28" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>324995</v>
+        <v>342075</v>
       </c>
       <c r="J28" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>8449865</v>
+        <v>8893940</v>
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
@@ -2149,7 +2179,7 @@
       </c>
       <c r="D29" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>8449865</v>
+        <v>8893940</v>
       </c>
       <c r="E29" s="14">
         <f t="shared" ca="1" si="5"/>
@@ -2165,15 +2195,15 @@
       </c>
       <c r="H29" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>9405052</v>
+        <v>9849127</v>
       </c>
       <c r="I29" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>376202</v>
+        <v>393965</v>
       </c>
       <c r="J29" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>9781254</v>
+        <v>10243092</v>
       </c>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
@@ -2187,7 +2217,7 @@
       </c>
       <c r="D30" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>9781254</v>
+        <v>10243092</v>
       </c>
       <c r="E30" s="14">
         <f t="shared" ca="1" si="5"/>
@@ -2203,15 +2233,15 @@
       </c>
       <c r="H30" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>10784200</v>
+        <v>11246038</v>
       </c>
       <c r="I30" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>431368</v>
+        <v>449842</v>
       </c>
       <c r="J30" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>11215568</v>
+        <v>11695880</v>
       </c>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
@@ -2225,7 +2255,7 @@
       </c>
       <c r="D31" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>11215568</v>
+        <v>11695880</v>
       </c>
       <c r="E31" s="14">
         <f t="shared" ca="1" si="5"/>
@@ -2241,15 +2271,15 @@
       </c>
       <c r="H31" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>12268661</v>
+        <v>12748973</v>
       </c>
       <c r="I31" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>490746</v>
+        <v>509959</v>
       </c>
       <c r="J31" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>12759407</v>
+        <v>13258932</v>
       </c>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
@@ -2263,7 +2293,7 @@
       </c>
       <c r="D32" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>12759407</v>
+        <v>13258932</v>
       </c>
       <c r="E32" s="14">
         <f t="shared" ca="1" si="5"/>
@@ -2279,15 +2309,15 @@
       </c>
       <c r="H32" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>13865155</v>
+        <v>14364680</v>
       </c>
       <c r="I32" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>554606</v>
+        <v>574587</v>
       </c>
       <c r="J32" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>14419761</v>
+        <v>14939267</v>
       </c>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
@@ -2301,7 +2331,7 @@
       </c>
       <c r="D33" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>14419761</v>
+        <v>14939267</v>
       </c>
       <c r="E33" s="14">
         <f t="shared" ca="1" si="5"/>
@@ -2317,15 +2347,15 @@
       </c>
       <c r="H33" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>15580796</v>
+        <v>16100302</v>
       </c>
       <c r="I33" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>623232</v>
+        <v>644012</v>
       </c>
       <c r="J33" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>16204028</v>
+        <v>16744314</v>
       </c>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
@@ -2339,7 +2369,7 @@
       </c>
       <c r="D34" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>16204028</v>
+        <v>16744314</v>
       </c>
       <c r="E34" s="14">
         <f t="shared" ca="1" si="5"/>
@@ -2355,15 +2385,15 @@
       </c>
       <c r="H34" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>17423115</v>
+        <v>17963401</v>
       </c>
       <c r="I34" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>696925</v>
+        <v>718536</v>
       </c>
       <c r="J34" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>18120040</v>
+        <v>18681937</v>
       </c>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
@@ -2377,7 +2407,7 @@
       </c>
       <c r="D35" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>18120040</v>
+        <v>18681937</v>
       </c>
       <c r="E35" s="14">
         <f t="shared" ca="1" si="5"/>
@@ -2393,15 +2423,15 @@
       </c>
       <c r="H35" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>19400081</v>
+        <v>19961978</v>
       </c>
       <c r="I35" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>776003</v>
+        <v>798479</v>
       </c>
       <c r="J35" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>20176084</v>
+        <v>20760457</v>
       </c>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
@@ -2415,7 +2445,7 @@
       </c>
       <c r="D36" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>20176084</v>
+        <v>20760457</v>
       </c>
       <c r="E36" s="14">
         <f t="shared" ca="1" si="5"/>
@@ -2431,15 +2461,15 @@
       </c>
       <c r="H36" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>21520127</v>
+        <v>22104500</v>
       </c>
       <c r="I36" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>860805</v>
+        <v>884180</v>
       </c>
       <c r="J36" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>22380932</v>
+        <v>22988680</v>
       </c>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
@@ -2453,7 +2483,7 @@
       </c>
       <c r="D37" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>22380932</v>
+        <v>22988680</v>
       </c>
       <c r="E37" s="14">
         <f t="shared" ca="1" si="5"/>
@@ -2469,15 +2499,15 @@
       </c>
       <c r="H37" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>23792177</v>
+        <v>24399925</v>
       </c>
       <c r="I37" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>951687</v>
+        <v>975997</v>
       </c>
       <c r="J37" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>24743864</v>
+        <v>25375922</v>
       </c>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
@@ -2491,7 +2521,7 @@
       </c>
       <c r="D38" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>24743864</v>
+        <v>25375922</v>
       </c>
       <c r="E38" s="14">
         <f t="shared" ca="1" si="5"/>
@@ -2507,15 +2537,15 @@
       </c>
       <c r="H38" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>26225671</v>
+        <v>26857729</v>
       </c>
       <c r="I38" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>1049027</v>
+        <v>1074309</v>
       </c>
       <c r="J38" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>27274698</v>
+        <v>27932038</v>
       </c>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
@@ -2529,7 +2559,7 @@
       </c>
       <c r="D39" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>27274698</v>
+        <v>27932038</v>
       </c>
       <c r="E39" s="14">
         <f t="shared" ca="1" si="5"/>
@@ -2545,15 +2575,15 @@
       </c>
       <c r="H39" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>28830595</v>
+        <v>29487935</v>
       </c>
       <c r="I39" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>1153224</v>
+        <v>1179517</v>
       </c>
       <c r="J39" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>29983819</v>
+        <v>30667452</v>
       </c>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
@@ -2567,7 +2597,7 @@
       </c>
       <c r="D40" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>29983819</v>
+        <v>30667452</v>
       </c>
       <c r="E40" s="14">
         <f t="shared" ca="1" si="5"/>
@@ -2583,15 +2613,15 @@
       </c>
       <c r="H40" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>31617511</v>
+        <v>32301144</v>
       </c>
       <c r="I40" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>1264700</v>
+        <v>1292046</v>
       </c>
       <c r="J40" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>32882211</v>
+        <v>33593190</v>
       </c>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.25">
@@ -2605,7 +2635,7 @@
       </c>
       <c r="D41" s="5">
         <f t="shared" ca="1" si="4"/>
-        <v>32882211</v>
+        <v>33593190</v>
       </c>
       <c r="E41" s="14">
         <f t="shared" ca="1" si="5"/>
@@ -2621,15 +2651,15 @@
       </c>
       <c r="H41" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>34597588</v>
+        <v>35308567</v>
       </c>
       <c r="I41" s="5">
         <f t="shared" ref="I41:I72" ca="1" si="7">ROUND(IF($C41&gt;=userRetirementAge, IF($H41&gt;0, $H41*annualEffectivePostRetirementROI, 0), IF($H41&gt;0, $H41*annualEffectiveROI, 0)), 0)</f>
-        <v>1383904</v>
+        <v>1412343</v>
       </c>
       <c r="J41" s="6">
         <f t="shared" ref="J41:J72" ca="1" si="8">ROUND(H41+I41, 0)</f>
-        <v>35981492</v>
+        <v>36720910</v>
       </c>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
@@ -2643,7 +2673,7 @@
       </c>
       <c r="D42" s="5">
         <f t="shared" ref="D42:D73" ca="1" si="11">ROUND(J41, 0)</f>
-        <v>35981492</v>
+        <v>36720910</v>
       </c>
       <c r="E42" s="14">
         <f t="shared" ref="E42:E73" ca="1" si="12">ROUND(IF($C42&gt;userRetirementAge, IF($D42&gt;0,-FV(annualChangeInSWP, $C42-userRetirementAge-1, 0, -annualAmountSWP, 1), 0), E41+E41*(annualIncreaseInSavings)), 0)</f>
@@ -2659,15 +2689,15 @@
       </c>
       <c r="H42" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>37782638</v>
+        <v>38522056</v>
       </c>
       <c r="I42" s="5">
         <f t="shared" ca="1" si="7"/>
-        <v>1511306</v>
+        <v>1540882</v>
       </c>
       <c r="J42" s="6">
         <f t="shared" ca="1" si="8"/>
-        <v>39293944</v>
+        <v>40062938</v>
       </c>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.25">
@@ -2681,7 +2711,7 @@
       </c>
       <c r="D43" s="5">
         <f t="shared" ca="1" si="11"/>
-        <v>39293944</v>
+        <v>40062938</v>
       </c>
       <c r="E43" s="14">
         <f t="shared" ca="1" si="12"/>
@@ -2697,15 +2727,15 @@
       </c>
       <c r="H43" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>41185147</v>
+        <v>41954141</v>
       </c>
       <c r="I43" s="5">
         <f t="shared" ca="1" si="7"/>
-        <v>1647406</v>
+        <v>1678166</v>
       </c>
       <c r="J43" s="6">
         <f t="shared" ca="1" si="8"/>
-        <v>42832553</v>
+        <v>43632307</v>
       </c>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.25">
@@ -2719,7 +2749,7 @@
       </c>
       <c r="D44" s="5">
         <f t="shared" ca="1" si="11"/>
-        <v>42832553</v>
+        <v>43632307</v>
       </c>
       <c r="E44" s="14">
         <f t="shared" ca="1" si="12"/>
@@ -2727,23 +2757,23 @@
       </c>
       <c r="F44" s="4">
         <f ca="1">-SUMIFS('Input-Events'!F$4:F$106, 'Input-Events'!E$4:E$106, $C44)</f>
-        <v>-700000</v>
+        <v>500000</v>
       </c>
       <c r="G44" s="4" t="str" cm="1">
         <f t="array" aca="1" ref="G44" ca="1">_xlfn.TEXTJOIN(", ", TRUE, IF('Input-Events'!E$4:E$106=$C44, 'Input-Events'!D$4:D$106, ""))</f>
-        <v>International Trip, Retirement</v>
+        <v>International Trip, Retirement Corpus, Retirement</v>
       </c>
       <c r="H44" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>44118316</v>
+        <v>46118070</v>
       </c>
       <c r="I44" s="5">
         <f t="shared" ca="1" si="7"/>
-        <v>441183</v>
+        <v>922361</v>
       </c>
       <c r="J44" s="6">
         <f t="shared" ca="1" si="8"/>
-        <v>44559499</v>
+        <v>47040431</v>
       </c>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.25">
@@ -2757,7 +2787,7 @@
       </c>
       <c r="D45" s="5">
         <f t="shared" ca="1" si="11"/>
-        <v>44559499</v>
+        <v>47040431</v>
       </c>
       <c r="E45" s="14">
         <f t="shared" ca="1" si="12"/>
@@ -2773,15 +2803,15 @@
       </c>
       <c r="H45" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>43359499</v>
+        <v>45840431</v>
       </c>
       <c r="I45" s="5">
         <f t="shared" ca="1" si="7"/>
-        <v>433595</v>
+        <v>916809</v>
       </c>
       <c r="J45" s="6">
         <f t="shared" ca="1" si="8"/>
-        <v>43793094</v>
+        <v>46757240</v>
       </c>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.25">
@@ -2795,7 +2825,7 @@
       </c>
       <c r="D46" s="5">
         <f t="shared" ca="1" si="11"/>
-        <v>43793094</v>
+        <v>46757240</v>
       </c>
       <c r="E46" s="14">
         <f t="shared" ca="1" si="12"/>
@@ -2811,15 +2841,15 @@
       </c>
       <c r="H46" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>42533094</v>
+        <v>45497240</v>
       </c>
       <c r="I46" s="5">
         <f t="shared" ca="1" si="7"/>
-        <v>425331</v>
+        <v>909945</v>
       </c>
       <c r="J46" s="6">
         <f t="shared" ca="1" si="8"/>
-        <v>42958425</v>
+        <v>46407185</v>
       </c>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.25">
@@ -2833,7 +2863,7 @@
       </c>
       <c r="D47" s="5">
         <f t="shared" ca="1" si="11"/>
-        <v>42958425</v>
+        <v>46407185</v>
       </c>
       <c r="E47" s="14">
         <f t="shared" ca="1" si="12"/>
@@ -2849,15 +2879,15 @@
       </c>
       <c r="H47" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>41635425</v>
+        <v>45084185</v>
       </c>
       <c r="I47" s="5">
         <f t="shared" ca="1" si="7"/>
-        <v>416354</v>
+        <v>901684</v>
       </c>
       <c r="J47" s="6">
         <f t="shared" ca="1" si="8"/>
-        <v>42051779</v>
+        <v>45985869</v>
       </c>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.25">
@@ -2871,7 +2901,7 @@
       </c>
       <c r="D48" s="5">
         <f t="shared" ca="1" si="11"/>
-        <v>42051779</v>
+        <v>45985869</v>
       </c>
       <c r="E48" s="14">
         <f t="shared" ca="1" si="12"/>
@@ -2887,15 +2917,15 @@
       </c>
       <c r="H48" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>40662629</v>
+        <v>44596719</v>
       </c>
       <c r="I48" s="5">
         <f t="shared" ca="1" si="7"/>
-        <v>406626</v>
+        <v>891934</v>
       </c>
       <c r="J48" s="6">
         <f t="shared" ca="1" si="8"/>
-        <v>41069255</v>
+        <v>45488653</v>
       </c>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.25">
@@ -2909,7 +2939,7 @@
       </c>
       <c r="D49" s="5">
         <f t="shared" ca="1" si="11"/>
-        <v>41069255</v>
+        <v>45488653</v>
       </c>
       <c r="E49" s="14">
         <f t="shared" ca="1" si="12"/>
@@ -2925,15 +2955,15 @@
       </c>
       <c r="H49" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>39610647</v>
+        <v>44030045</v>
       </c>
       <c r="I49" s="5">
         <f t="shared" ca="1" si="7"/>
-        <v>396106</v>
+        <v>880601</v>
       </c>
       <c r="J49" s="6">
         <f t="shared" ca="1" si="8"/>
-        <v>40006753</v>
+        <v>44910646</v>
       </c>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.25">
@@ -2947,7 +2977,7 @@
       </c>
       <c r="D50" s="5">
         <f t="shared" ca="1" si="11"/>
-        <v>40006753</v>
+        <v>44910646</v>
       </c>
       <c r="E50" s="14">
         <f t="shared" ca="1" si="12"/>
@@ -2963,15 +2993,15 @@
       </c>
       <c r="H50" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>38475215</v>
+        <v>43379108</v>
       </c>
       <c r="I50" s="5">
         <f t="shared" ca="1" si="7"/>
-        <v>384752</v>
+        <v>867582</v>
       </c>
       <c r="J50" s="6">
         <f t="shared" ca="1" si="8"/>
-        <v>38859967</v>
+        <v>44246690</v>
       </c>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.25">
@@ -2985,7 +3015,7 @@
       </c>
       <c r="D51" s="5">
         <f t="shared" ca="1" si="11"/>
-        <v>38859967</v>
+        <v>44246690</v>
       </c>
       <c r="E51" s="14">
         <f t="shared" ca="1" si="12"/>
@@ -3001,15 +3031,15 @@
       </c>
       <c r="H51" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>37251852</v>
+        <v>42638575</v>
       </c>
       <c r="I51" s="5">
         <f t="shared" ca="1" si="7"/>
-        <v>372519</v>
+        <v>852772</v>
       </c>
       <c r="J51" s="6">
         <f t="shared" ca="1" si="8"/>
-        <v>37624371</v>
+        <v>43491347</v>
       </c>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.25">
@@ -3023,7 +3053,7 @@
       </c>
       <c r="D52" s="5">
         <f t="shared" ca="1" si="11"/>
-        <v>37624371</v>
+        <v>43491347</v>
       </c>
       <c r="E52" s="14">
         <f t="shared" ca="1" si="12"/>
@@ -3039,15 +3069,15 @@
       </c>
       <c r="H52" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>35935850</v>
+        <v>41802826</v>
       </c>
       <c r="I52" s="5">
         <f t="shared" ca="1" si="7"/>
-        <v>359359</v>
+        <v>836057</v>
       </c>
       <c r="J52" s="6">
         <f t="shared" ca="1" si="8"/>
-        <v>36295209</v>
+        <v>42638883</v>
       </c>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.25">
@@ -3061,7 +3091,7 @@
       </c>
       <c r="D53" s="5">
         <f t="shared" ca="1" si="11"/>
-        <v>36295209</v>
+        <v>42638883</v>
       </c>
       <c r="E53" s="14">
         <f t="shared" ca="1" si="12"/>
@@ -3077,15 +3107,15 @@
       </c>
       <c r="H53" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>34522262</v>
+        <v>40865936</v>
       </c>
       <c r="I53" s="5">
         <f t="shared" ca="1" si="7"/>
-        <v>345223</v>
+        <v>817319</v>
       </c>
       <c r="J53" s="6">
         <f t="shared" ca="1" si="8"/>
-        <v>34867485</v>
+        <v>41683255</v>
       </c>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.25">
@@ -3099,7 +3129,7 @@
       </c>
       <c r="D54" s="5">
         <f t="shared" ca="1" si="11"/>
-        <v>34867485</v>
+        <v>41683255</v>
       </c>
       <c r="E54" s="14">
         <f t="shared" ca="1" si="12"/>
@@ -3115,15 +3145,15 @@
       </c>
       <c r="H54" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>33005891</v>
+        <v>39821661</v>
       </c>
       <c r="I54" s="5">
         <f t="shared" ca="1" si="7"/>
-        <v>330059</v>
+        <v>796433</v>
       </c>
       <c r="J54" s="6">
         <f t="shared" ca="1" si="8"/>
-        <v>33335950</v>
+        <v>40618094</v>
       </c>
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.25">
@@ -3137,7 +3167,7 @@
       </c>
       <c r="D55" s="5">
         <f t="shared" ca="1" si="11"/>
-        <v>33335950</v>
+        <v>40618094</v>
       </c>
       <c r="E55" s="14">
         <f t="shared" ca="1" si="12"/>
@@ -3153,15 +3183,15 @@
       </c>
       <c r="H55" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>31381276</v>
+        <v>38663420</v>
       </c>
       <c r="I55" s="5">
         <f t="shared" ca="1" si="7"/>
-        <v>313813</v>
+        <v>773268</v>
       </c>
       <c r="J55" s="6">
         <f t="shared" ca="1" si="8"/>
-        <v>31695089</v>
+        <v>39436688</v>
       </c>
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.25">
@@ -3175,7 +3205,7 @@
       </c>
       <c r="D56" s="5">
         <f t="shared" ca="1" si="11"/>
-        <v>31695089</v>
+        <v>39436688</v>
       </c>
       <c r="E56" s="14">
         <f t="shared" ca="1" si="12"/>
@@ -3191,15 +3221,15 @@
       </c>
       <c r="H56" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>29642682</v>
+        <v>37384281</v>
       </c>
       <c r="I56" s="5">
         <f t="shared" ca="1" si="7"/>
-        <v>296427</v>
+        <v>747686</v>
       </c>
       <c r="J56" s="6">
         <f t="shared" ca="1" si="8"/>
-        <v>29939109</v>
+        <v>38131967</v>
       </c>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.25">
@@ -3213,7 +3243,7 @@
       </c>
       <c r="D57" s="5">
         <f t="shared" ca="1" si="11"/>
-        <v>29939109</v>
+        <v>38131967</v>
       </c>
       <c r="E57" s="14">
         <f t="shared" ca="1" si="12"/>
@@ -3229,15 +3259,15 @@
       </c>
       <c r="H57" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>27784081</v>
+        <v>35976939</v>
       </c>
       <c r="I57" s="5">
         <f t="shared" ca="1" si="7"/>
-        <v>277841</v>
+        <v>719539</v>
       </c>
       <c r="J57" s="6">
         <f t="shared" ca="1" si="8"/>
-        <v>28061922</v>
+        <v>36696478</v>
       </c>
     </row>
     <row r="58" spans="2:10" x14ac:dyDescent="0.25">
@@ -3251,7 +3281,7 @@
       </c>
       <c r="D58" s="5">
         <f t="shared" ca="1" si="11"/>
-        <v>28061922</v>
+        <v>36696478</v>
       </c>
       <c r="E58" s="14">
         <f t="shared" ca="1" si="12"/>
@@ -3267,15 +3297,15 @@
       </c>
       <c r="H58" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>25799143</v>
+        <v>34433699</v>
       </c>
       <c r="I58" s="5">
         <f t="shared" ca="1" si="7"/>
-        <v>257991</v>
+        <v>688674</v>
       </c>
       <c r="J58" s="6">
         <f t="shared" ca="1" si="8"/>
-        <v>26057134</v>
+        <v>35122373</v>
       </c>
     </row>
     <row r="59" spans="2:10" x14ac:dyDescent="0.25">
@@ -3289,7 +3319,7 @@
       </c>
       <c r="D59" s="5">
         <f t="shared" ca="1" si="11"/>
-        <v>26057134</v>
+        <v>35122373</v>
       </c>
       <c r="E59" s="14">
         <f t="shared" ca="1" si="12"/>
@@ -3305,15 +3335,15 @@
       </c>
       <c r="H59" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>23681216</v>
+        <v>32746455</v>
       </c>
       <c r="I59" s="5">
         <f t="shared" ca="1" si="7"/>
-        <v>236812</v>
+        <v>654929</v>
       </c>
       <c r="J59" s="6">
         <f t="shared" ca="1" si="8"/>
-        <v>23918028</v>
+        <v>33401384</v>
       </c>
     </row>
     <row r="60" spans="2:10" x14ac:dyDescent="0.25">
@@ -3327,7 +3357,7 @@
       </c>
       <c r="D60" s="5">
         <f t="shared" ca="1" si="11"/>
-        <v>23918028</v>
+        <v>33401384</v>
       </c>
       <c r="E60" s="14">
         <f t="shared" ca="1" si="12"/>
@@ -3343,15 +3373,15 @@
       </c>
       <c r="H60" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>21423314</v>
+        <v>30906670</v>
       </c>
       <c r="I60" s="5">
         <f t="shared" ca="1" si="7"/>
-        <v>214233</v>
+        <v>618133</v>
       </c>
       <c r="J60" s="6">
         <f t="shared" ca="1" si="8"/>
-        <v>21637547</v>
+        <v>31524803</v>
       </c>
     </row>
     <row r="61" spans="2:10" x14ac:dyDescent="0.25">
@@ -3365,7 +3395,7 @@
       </c>
       <c r="D61" s="5">
         <f t="shared" ca="1" si="11"/>
-        <v>21637547</v>
+        <v>31524803</v>
       </c>
       <c r="E61" s="14">
         <f t="shared" ca="1" si="12"/>
@@ -3381,15 +3411,15 @@
       </c>
       <c r="H61" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>19018097</v>
+        <v>28905353</v>
       </c>
       <c r="I61" s="5">
         <f t="shared" ca="1" si="7"/>
-        <v>190181</v>
+        <v>578107</v>
       </c>
       <c r="J61" s="6">
         <f t="shared" ca="1" si="8"/>
-        <v>19208278</v>
+        <v>29483460</v>
       </c>
     </row>
     <row r="62" spans="2:10" x14ac:dyDescent="0.25">
@@ -3403,7 +3433,7 @@
       </c>
       <c r="D62" s="5">
         <f t="shared" ca="1" si="11"/>
-        <v>19208278</v>
+        <v>29483460</v>
       </c>
       <c r="E62" s="14">
         <f t="shared" ca="1" si="12"/>
@@ -3419,15 +3449,15 @@
       </c>
       <c r="H62" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>16457856</v>
+        <v>26733038</v>
       </c>
       <c r="I62" s="5">
         <f t="shared" ca="1" si="7"/>
-        <v>164579</v>
+        <v>534661</v>
       </c>
       <c r="J62" s="6">
         <f t="shared" ca="1" si="8"/>
-        <v>16622435</v>
+        <v>27267699</v>
       </c>
     </row>
     <row r="63" spans="2:10" x14ac:dyDescent="0.25">
@@ -3441,7 +3471,7 @@
       </c>
       <c r="D63" s="5">
         <f t="shared" ca="1" si="11"/>
-        <v>16622435</v>
+        <v>27267699</v>
       </c>
       <c r="E63" s="14">
         <f t="shared" ca="1" si="12"/>
@@ -3457,15 +3487,15 @@
       </c>
       <c r="H63" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>13734492</v>
+        <v>24379756</v>
       </c>
       <c r="I63" s="5">
         <f t="shared" ca="1" si="7"/>
-        <v>137345</v>
+        <v>487595</v>
       </c>
       <c r="J63" s="6">
         <f t="shared" ca="1" si="8"/>
-        <v>13871837</v>
+        <v>24867351</v>
       </c>
     </row>
     <row r="64" spans="2:10" x14ac:dyDescent="0.25">
@@ -3479,7 +3509,7 @@
       </c>
       <c r="D64" s="5">
         <f t="shared" ca="1" si="11"/>
-        <v>13871837</v>
+        <v>24867351</v>
       </c>
       <c r="E64" s="14">
         <f t="shared" ca="1" si="12"/>
@@ -3495,15 +3525,15 @@
       </c>
       <c r="H64" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>20839497</v>
+        <v>31835011</v>
       </c>
       <c r="I64" s="5">
         <f t="shared" ca="1" si="7"/>
-        <v>208395</v>
+        <v>636700</v>
       </c>
       <c r="J64" s="6">
         <f t="shared" ca="1" si="8"/>
-        <v>21047892</v>
+        <v>32471711</v>
       </c>
     </row>
     <row r="65" spans="2:10" x14ac:dyDescent="0.25">
@@ -3517,7 +3547,7 @@
       </c>
       <c r="D65" s="5">
         <f t="shared" ca="1" si="11"/>
-        <v>21047892</v>
+        <v>32471711</v>
       </c>
       <c r="E65" s="14">
         <f t="shared" ca="1" si="12"/>
@@ -3533,15 +3563,15 @@
       </c>
       <c r="H65" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>17863935</v>
+        <v>29287754</v>
       </c>
       <c r="I65" s="5">
         <f t="shared" ca="1" si="7"/>
-        <v>178639</v>
+        <v>585755</v>
       </c>
       <c r="J65" s="6">
         <f t="shared" ca="1" si="8"/>
-        <v>18042574</v>
+        <v>29873509</v>
       </c>
     </row>
     <row r="66" spans="2:10" x14ac:dyDescent="0.25">
@@ -3555,7 +3585,7 @@
       </c>
       <c r="D66" s="5">
         <f t="shared" ca="1" si="11"/>
-        <v>18042574</v>
+        <v>29873509</v>
       </c>
       <c r="E66" s="14">
         <f t="shared" ca="1" si="12"/>
@@ -3571,15 +3601,15 @@
       </c>
       <c r="H66" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>14699419</v>
+        <v>26530354</v>
       </c>
       <c r="I66" s="5">
         <f t="shared" ca="1" si="7"/>
-        <v>146994</v>
+        <v>530607</v>
       </c>
       <c r="J66" s="6">
         <f t="shared" ca="1" si="8"/>
-        <v>14846413</v>
+        <v>27060961</v>
       </c>
     </row>
     <row r="67" spans="2:10" x14ac:dyDescent="0.25">
@@ -3593,7 +3623,7 @@
       </c>
       <c r="D67" s="5">
         <f t="shared" ca="1" si="11"/>
-        <v>14846413</v>
+        <v>27060961</v>
       </c>
       <c r="E67" s="14">
         <f t="shared" ca="1" si="12"/>
@@ -3609,15 +3639,15 @@
       </c>
       <c r="H67" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>11336100</v>
+        <v>23550648</v>
       </c>
       <c r="I67" s="5">
         <f t="shared" ca="1" si="7"/>
-        <v>113361</v>
+        <v>471013</v>
       </c>
       <c r="J67" s="6">
         <f t="shared" ca="1" si="8"/>
-        <v>11449461</v>
+        <v>24021661</v>
       </c>
     </row>
     <row r="68" spans="2:10" x14ac:dyDescent="0.25">
@@ -3631,7 +3661,7 @@
       </c>
       <c r="D68" s="5">
         <f t="shared" ca="1" si="11"/>
-        <v>11449461</v>
+        <v>24021661</v>
       </c>
       <c r="E68" s="14">
         <f t="shared" ca="1" si="12"/>
@@ -3647,15 +3677,15 @@
       </c>
       <c r="H68" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>7763632</v>
+        <v>20335832</v>
       </c>
       <c r="I68" s="5">
         <f t="shared" ca="1" si="7"/>
-        <v>77636</v>
+        <v>406717</v>
       </c>
       <c r="J68" s="6">
         <f t="shared" ca="1" si="8"/>
-        <v>7841268</v>
+        <v>20742549</v>
       </c>
     </row>
     <row r="69" spans="2:10" x14ac:dyDescent="0.25">
@@ -3669,7 +3699,7 @@
       </c>
       <c r="D69" s="5">
         <f t="shared" ca="1" si="11"/>
-        <v>7841268</v>
+        <v>20742549</v>
       </c>
       <c r="E69" s="14">
         <f t="shared" ca="1" si="12"/>
@@ -3685,15 +3715,15 @@
       </c>
       <c r="H69" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>3971148</v>
+        <v>16872429</v>
       </c>
       <c r="I69" s="5">
         <f t="shared" ca="1" si="7"/>
-        <v>39711</v>
+        <v>337449</v>
       </c>
       <c r="J69" s="6">
         <f t="shared" ca="1" si="8"/>
-        <v>4010859</v>
+        <v>17209878</v>
       </c>
     </row>
     <row r="70" spans="2:10" x14ac:dyDescent="0.25">
@@ -3707,7 +3737,7 @@
       </c>
       <c r="D70" s="5">
         <f t="shared" ca="1" si="11"/>
-        <v>4010859</v>
+        <v>17209878</v>
       </c>
       <c r="E70" s="14">
         <f t="shared" ca="1" si="12"/>
@@ -3723,15 +3753,15 @@
       </c>
       <c r="H70" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>-52767</v>
+        <v>13146252</v>
       </c>
       <c r="I70" s="5">
         <f t="shared" ca="1" si="7"/>
-        <v>0</v>
+        <v>262925</v>
       </c>
       <c r="J70" s="6">
         <f t="shared" ca="1" si="8"/>
-        <v>-52767</v>
+        <v>13409177</v>
       </c>
     </row>
     <row r="71" spans="2:10" x14ac:dyDescent="0.25">
@@ -3745,11 +3775,11 @@
       </c>
       <c r="D71" s="5">
         <f t="shared" ca="1" si="11"/>
-        <v>-52767</v>
+        <v>13409177</v>
       </c>
       <c r="E71" s="14">
         <f t="shared" ca="1" si="12"/>
-        <v>0</v>
+        <v>-4266807</v>
       </c>
       <c r="F71" s="4">
         <f ca="1">-SUMIFS('Input-Events'!F$4:F$106, 'Input-Events'!E$4:E$106, $C71)</f>
@@ -3761,15 +3791,15 @@
       </c>
       <c r="H71" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>-52767</v>
+        <v>9142370</v>
       </c>
       <c r="I71" s="5">
         <f t="shared" ca="1" si="7"/>
-        <v>0</v>
+        <v>182847</v>
       </c>
       <c r="J71" s="6">
         <f t="shared" ca="1" si="8"/>
-        <v>-52767</v>
+        <v>9325217</v>
       </c>
     </row>
     <row r="72" spans="2:10" x14ac:dyDescent="0.25">
@@ -3783,11 +3813,11 @@
       </c>
       <c r="D72" s="5">
         <f t="shared" ca="1" si="11"/>
-        <v>-52767</v>
+        <v>9325217</v>
       </c>
       <c r="E72" s="14">
         <f t="shared" ca="1" si="12"/>
-        <v>0</v>
+        <v>-4480148</v>
       </c>
       <c r="F72" s="4">
         <f ca="1">-SUMIFS('Input-Events'!F$4:F$106, 'Input-Events'!E$4:E$106, $C72)</f>
@@ -3799,15 +3829,15 @@
       </c>
       <c r="H72" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>-52767</v>
+        <v>4845069</v>
       </c>
       <c r="I72" s="5">
         <f t="shared" ca="1" si="7"/>
-        <v>0</v>
+        <v>96901</v>
       </c>
       <c r="J72" s="6">
         <f t="shared" ca="1" si="8"/>
-        <v>-52767</v>
+        <v>4941970</v>
       </c>
     </row>
     <row r="73" spans="2:10" x14ac:dyDescent="0.25">
@@ -3821,11 +3851,11 @@
       </c>
       <c r="D73" s="5">
         <f t="shared" ca="1" si="11"/>
-        <v>-52767</v>
+        <v>4941970</v>
       </c>
       <c r="E73" s="14">
         <f t="shared" ca="1" si="12"/>
-        <v>0</v>
+        <v>-4704155</v>
       </c>
       <c r="F73" s="4">
         <f ca="1">-SUMIFS('Input-Events'!F$4:F$106, 'Input-Events'!E$4:E$106, $C73)</f>
@@ -3837,15 +3867,15 @@
       </c>
       <c r="H73" s="5">
         <f t="shared" ca="1" si="6"/>
-        <v>-52767</v>
+        <v>237815</v>
       </c>
       <c r="I73" s="5">
         <f t="shared" ref="I73:I109" ca="1" si="13">ROUND(IF($C73&gt;=userRetirementAge, IF($H73&gt;0, $H73*annualEffectivePostRetirementROI, 0), IF($H73&gt;0, $H73*annualEffectiveROI, 0)), 0)</f>
-        <v>0</v>
+        <v>4756</v>
       </c>
       <c r="J73" s="6">
         <f t="shared" ref="J73:J104" ca="1" si="14">ROUND(H73+I73, 0)</f>
-        <v>-52767</v>
+        <v>242571</v>
       </c>
     </row>
     <row r="74" spans="2:10" x14ac:dyDescent="0.25">
@@ -3859,11 +3889,11 @@
       </c>
       <c r="D74" s="5">
         <f t="shared" ref="D74:D109" ca="1" si="17">ROUND(J73, 0)</f>
-        <v>-52767</v>
+        <v>242571</v>
       </c>
       <c r="E74" s="14">
         <f t="shared" ref="E74:E109" ca="1" si="18">ROUND(IF($C74&gt;userRetirementAge, IF($D74&gt;0,-FV(annualChangeInSWP, $C74-userRetirementAge-1, 0, -annualAmountSWP, 1), 0), E73+E73*(annualIncreaseInSavings)), 0)</f>
-        <v>0</v>
+        <v>-4939363</v>
       </c>
       <c r="F74" s="4">
         <f ca="1">-SUMIFS('Input-Events'!F$4:F$106, 'Input-Events'!E$4:E$106, $C74)</f>
@@ -3875,7 +3905,7 @@
       </c>
       <c r="H74" s="5">
         <f t="shared" ref="H74:H109" ca="1" si="19">$D74+$E74+$F74</f>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="I74" s="5">
         <f t="shared" ca="1" si="13"/>
@@ -3883,7 +3913,7 @@
       </c>
       <c r="J74" s="6">
         <f t="shared" ca="1" si="14"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
     </row>
     <row r="75" spans="2:10" x14ac:dyDescent="0.25">
@@ -3897,7 +3927,7 @@
       </c>
       <c r="D75" s="5">
         <f t="shared" ca="1" si="17"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="E75" s="14">
         <f t="shared" ca="1" si="18"/>
@@ -3913,7 +3943,7 @@
       </c>
       <c r="H75" s="5">
         <f t="shared" ca="1" si="19"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="I75" s="5">
         <f t="shared" ca="1" si="13"/>
@@ -3921,7 +3951,7 @@
       </c>
       <c r="J75" s="6">
         <f t="shared" ca="1" si="14"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
     </row>
     <row r="76" spans="2:10" x14ac:dyDescent="0.25">
@@ -3935,7 +3965,7 @@
       </c>
       <c r="D76" s="5">
         <f t="shared" ca="1" si="17"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="E76" s="14">
         <f t="shared" ca="1" si="18"/>
@@ -3951,7 +3981,7 @@
       </c>
       <c r="H76" s="5">
         <f t="shared" ca="1" si="19"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="I76" s="5">
         <f t="shared" ca="1" si="13"/>
@@ -3959,7 +3989,7 @@
       </c>
       <c r="J76" s="6">
         <f t="shared" ca="1" si="14"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
     </row>
     <row r="77" spans="2:10" x14ac:dyDescent="0.25">
@@ -3973,7 +4003,7 @@
       </c>
       <c r="D77" s="5">
         <f t="shared" ca="1" si="17"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="E77" s="14">
         <f t="shared" ca="1" si="18"/>
@@ -3989,7 +4019,7 @@
       </c>
       <c r="H77" s="5">
         <f t="shared" ca="1" si="19"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="I77" s="5">
         <f t="shared" ca="1" si="13"/>
@@ -3997,7 +4027,7 @@
       </c>
       <c r="J77" s="6">
         <f t="shared" ca="1" si="14"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
     </row>
     <row r="78" spans="2:10" x14ac:dyDescent="0.25">
@@ -4011,7 +4041,7 @@
       </c>
       <c r="D78" s="5">
         <f t="shared" ca="1" si="17"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="E78" s="14">
         <f t="shared" ca="1" si="18"/>
@@ -4027,7 +4057,7 @@
       </c>
       <c r="H78" s="5">
         <f t="shared" ca="1" si="19"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="I78" s="5">
         <f t="shared" ca="1" si="13"/>
@@ -4035,7 +4065,7 @@
       </c>
       <c r="J78" s="6">
         <f t="shared" ca="1" si="14"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
     </row>
     <row r="79" spans="2:10" x14ac:dyDescent="0.25">
@@ -4049,7 +4079,7 @@
       </c>
       <c r="D79" s="5">
         <f t="shared" ca="1" si="17"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="E79" s="14">
         <f t="shared" ca="1" si="18"/>
@@ -4065,7 +4095,7 @@
       </c>
       <c r="H79" s="5">
         <f t="shared" ca="1" si="19"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="I79" s="5">
         <f t="shared" ca="1" si="13"/>
@@ -4073,7 +4103,7 @@
       </c>
       <c r="J79" s="6">
         <f t="shared" ca="1" si="14"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
     </row>
     <row r="80" spans="2:10" x14ac:dyDescent="0.25">
@@ -4087,7 +4117,7 @@
       </c>
       <c r="D80" s="5">
         <f t="shared" ca="1" si="17"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="E80" s="14">
         <f t="shared" ca="1" si="18"/>
@@ -4103,7 +4133,7 @@
       </c>
       <c r="H80" s="5">
         <f t="shared" ca="1" si="19"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="I80" s="5">
         <f t="shared" ca="1" si="13"/>
@@ -4111,7 +4141,7 @@
       </c>
       <c r="J80" s="6">
         <f t="shared" ca="1" si="14"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
     </row>
     <row r="81" spans="2:10" x14ac:dyDescent="0.25">
@@ -4125,7 +4155,7 @@
       </c>
       <c r="D81" s="5">
         <f t="shared" ca="1" si="17"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="E81" s="14">
         <f t="shared" ca="1" si="18"/>
@@ -4141,7 +4171,7 @@
       </c>
       <c r="H81" s="5">
         <f t="shared" ca="1" si="19"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="I81" s="5">
         <f t="shared" ca="1" si="13"/>
@@ -4149,7 +4179,7 @@
       </c>
       <c r="J81" s="6">
         <f t="shared" ca="1" si="14"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
     </row>
     <row r="82" spans="2:10" x14ac:dyDescent="0.25">
@@ -4163,7 +4193,7 @@
       </c>
       <c r="D82" s="5">
         <f t="shared" ca="1" si="17"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="E82" s="14">
         <f t="shared" ca="1" si="18"/>
@@ -4179,7 +4209,7 @@
       </c>
       <c r="H82" s="5">
         <f t="shared" ca="1" si="19"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="I82" s="5">
         <f t="shared" ca="1" si="13"/>
@@ -4187,7 +4217,7 @@
       </c>
       <c r="J82" s="6">
         <f t="shared" ca="1" si="14"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
     </row>
     <row r="83" spans="2:10" x14ac:dyDescent="0.25">
@@ -4201,7 +4231,7 @@
       </c>
       <c r="D83" s="5">
         <f t="shared" ca="1" si="17"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="E83" s="14">
         <f t="shared" ca="1" si="18"/>
@@ -4217,7 +4247,7 @@
       </c>
       <c r="H83" s="5">
         <f t="shared" ca="1" si="19"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="I83" s="5">
         <f t="shared" ca="1" si="13"/>
@@ -4225,7 +4255,7 @@
       </c>
       <c r="J83" s="6">
         <f t="shared" ca="1" si="14"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
     </row>
     <row r="84" spans="2:10" x14ac:dyDescent="0.25">
@@ -4239,7 +4269,7 @@
       </c>
       <c r="D84" s="5">
         <f t="shared" ca="1" si="17"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="E84" s="14">
         <f t="shared" ca="1" si="18"/>
@@ -4255,7 +4285,7 @@
       </c>
       <c r="H84" s="5">
         <f t="shared" ca="1" si="19"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="I84" s="5">
         <f t="shared" ca="1" si="13"/>
@@ -4263,7 +4293,7 @@
       </c>
       <c r="J84" s="6">
         <f t="shared" ca="1" si="14"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
     </row>
     <row r="85" spans="2:10" x14ac:dyDescent="0.25">
@@ -4277,7 +4307,7 @@
       </c>
       <c r="D85" s="5">
         <f t="shared" ca="1" si="17"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="E85" s="14">
         <f t="shared" ca="1" si="18"/>
@@ -4293,7 +4323,7 @@
       </c>
       <c r="H85" s="5">
         <f t="shared" ca="1" si="19"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="I85" s="5">
         <f t="shared" ca="1" si="13"/>
@@ -4301,7 +4331,7 @@
       </c>
       <c r="J85" s="6">
         <f t="shared" ca="1" si="14"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
     </row>
     <row r="86" spans="2:10" x14ac:dyDescent="0.25">
@@ -4315,7 +4345,7 @@
       </c>
       <c r="D86" s="5">
         <f t="shared" ca="1" si="17"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="E86" s="14">
         <f t="shared" ca="1" si="18"/>
@@ -4331,7 +4361,7 @@
       </c>
       <c r="H86" s="5">
         <f t="shared" ca="1" si="19"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="I86" s="5">
         <f t="shared" ca="1" si="13"/>
@@ -4339,7 +4369,7 @@
       </c>
       <c r="J86" s="6">
         <f t="shared" ca="1" si="14"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
     </row>
     <row r="87" spans="2:10" x14ac:dyDescent="0.25">
@@ -4353,7 +4383,7 @@
       </c>
       <c r="D87" s="5">
         <f t="shared" ca="1" si="17"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="E87" s="14">
         <f t="shared" ca="1" si="18"/>
@@ -4369,7 +4399,7 @@
       </c>
       <c r="H87" s="5">
         <f t="shared" ca="1" si="19"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="I87" s="5">
         <f t="shared" ca="1" si="13"/>
@@ -4377,7 +4407,7 @@
       </c>
       <c r="J87" s="6">
         <f t="shared" ca="1" si="14"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
     </row>
     <row r="88" spans="2:10" x14ac:dyDescent="0.25">
@@ -4391,7 +4421,7 @@
       </c>
       <c r="D88" s="5">
         <f t="shared" ca="1" si="17"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="E88" s="14">
         <f t="shared" ca="1" si="18"/>
@@ -4407,7 +4437,7 @@
       </c>
       <c r="H88" s="5">
         <f t="shared" ca="1" si="19"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="I88" s="5">
         <f t="shared" ca="1" si="13"/>
@@ -4415,7 +4445,7 @@
       </c>
       <c r="J88" s="6">
         <f t="shared" ca="1" si="14"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
     </row>
     <row r="89" spans="2:10" x14ac:dyDescent="0.25">
@@ -4429,7 +4459,7 @@
       </c>
       <c r="D89" s="5">
         <f t="shared" ca="1" si="17"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="E89" s="14">
         <f t="shared" ca="1" si="18"/>
@@ -4445,7 +4475,7 @@
       </c>
       <c r="H89" s="5">
         <f t="shared" ca="1" si="19"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="I89" s="5">
         <f t="shared" ca="1" si="13"/>
@@ -4453,7 +4483,7 @@
       </c>
       <c r="J89" s="6">
         <f t="shared" ca="1" si="14"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
     </row>
     <row r="90" spans="2:10" x14ac:dyDescent="0.25">
@@ -4467,7 +4497,7 @@
       </c>
       <c r="D90" s="5">
         <f t="shared" ca="1" si="17"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="E90" s="14">
         <f t="shared" ca="1" si="18"/>
@@ -4483,7 +4513,7 @@
       </c>
       <c r="H90" s="5">
         <f t="shared" ca="1" si="19"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="I90" s="5">
         <f t="shared" ca="1" si="13"/>
@@ -4491,7 +4521,7 @@
       </c>
       <c r="J90" s="6">
         <f t="shared" ca="1" si="14"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
     </row>
     <row r="91" spans="2:10" x14ac:dyDescent="0.25">
@@ -4505,7 +4535,7 @@
       </c>
       <c r="D91" s="5">
         <f t="shared" ca="1" si="17"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="E91" s="14">
         <f t="shared" ca="1" si="18"/>
@@ -4521,7 +4551,7 @@
       </c>
       <c r="H91" s="5">
         <f t="shared" ca="1" si="19"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="I91" s="5">
         <f t="shared" ca="1" si="13"/>
@@ -4529,7 +4559,7 @@
       </c>
       <c r="J91" s="6">
         <f t="shared" ca="1" si="14"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
     </row>
     <row r="92" spans="2:10" x14ac:dyDescent="0.25">
@@ -4543,7 +4573,7 @@
       </c>
       <c r="D92" s="5">
         <f t="shared" ca="1" si="17"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="E92" s="14">
         <f t="shared" ca="1" si="18"/>
@@ -4559,7 +4589,7 @@
       </c>
       <c r="H92" s="5">
         <f t="shared" ca="1" si="19"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="I92" s="5">
         <f t="shared" ca="1" si="13"/>
@@ -4567,7 +4597,7 @@
       </c>
       <c r="J92" s="6">
         <f t="shared" ca="1" si="14"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
     </row>
     <row r="93" spans="2:10" x14ac:dyDescent="0.25">
@@ -4581,7 +4611,7 @@
       </c>
       <c r="D93" s="5">
         <f t="shared" ca="1" si="17"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="E93" s="14">
         <f t="shared" ca="1" si="18"/>
@@ -4597,7 +4627,7 @@
       </c>
       <c r="H93" s="5">
         <f t="shared" ca="1" si="19"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="I93" s="5">
         <f t="shared" ca="1" si="13"/>
@@ -4605,7 +4635,7 @@
       </c>
       <c r="J93" s="6">
         <f t="shared" ca="1" si="14"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
     </row>
     <row r="94" spans="2:10" x14ac:dyDescent="0.25">
@@ -4619,7 +4649,7 @@
       </c>
       <c r="D94" s="5">
         <f t="shared" ca="1" si="17"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="E94" s="14">
         <f t="shared" ca="1" si="18"/>
@@ -4635,7 +4665,7 @@
       </c>
       <c r="H94" s="5">
         <f t="shared" ca="1" si="19"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="I94" s="5">
         <f t="shared" ca="1" si="13"/>
@@ -4643,7 +4673,7 @@
       </c>
       <c r="J94" s="6">
         <f t="shared" ca="1" si="14"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
     </row>
     <row r="95" spans="2:10" x14ac:dyDescent="0.25">
@@ -4657,7 +4687,7 @@
       </c>
       <c r="D95" s="5">
         <f t="shared" ca="1" si="17"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="E95" s="14">
         <f t="shared" ca="1" si="18"/>
@@ -4673,7 +4703,7 @@
       </c>
       <c r="H95" s="5">
         <f t="shared" ca="1" si="19"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="I95" s="5">
         <f t="shared" ca="1" si="13"/>
@@ -4681,7 +4711,7 @@
       </c>
       <c r="J95" s="6">
         <f t="shared" ca="1" si="14"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
     </row>
     <row r="96" spans="2:10" x14ac:dyDescent="0.25">
@@ -4695,7 +4725,7 @@
       </c>
       <c r="D96" s="5">
         <f t="shared" ca="1" si="17"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="E96" s="14">
         <f t="shared" ca="1" si="18"/>
@@ -4711,7 +4741,7 @@
       </c>
       <c r="H96" s="5">
         <f t="shared" ca="1" si="19"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="I96" s="5">
         <f t="shared" ca="1" si="13"/>
@@ -4719,7 +4749,7 @@
       </c>
       <c r="J96" s="6">
         <f t="shared" ca="1" si="14"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
     </row>
     <row r="97" spans="2:10" x14ac:dyDescent="0.25">
@@ -4733,7 +4763,7 @@
       </c>
       <c r="D97" s="5">
         <f t="shared" ca="1" si="17"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="E97" s="14">
         <f t="shared" ca="1" si="18"/>
@@ -4749,7 +4779,7 @@
       </c>
       <c r="H97" s="5">
         <f t="shared" ca="1" si="19"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="I97" s="5">
         <f t="shared" ca="1" si="13"/>
@@ -4757,7 +4787,7 @@
       </c>
       <c r="J97" s="6">
         <f t="shared" ca="1" si="14"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
     </row>
     <row r="98" spans="2:10" x14ac:dyDescent="0.25">
@@ -4771,7 +4801,7 @@
       </c>
       <c r="D98" s="5">
         <f t="shared" ca="1" si="17"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="E98" s="14">
         <f t="shared" ca="1" si="18"/>
@@ -4787,7 +4817,7 @@
       </c>
       <c r="H98" s="5">
         <f t="shared" ca="1" si="19"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="I98" s="5">
         <f t="shared" ca="1" si="13"/>
@@ -4795,7 +4825,7 @@
       </c>
       <c r="J98" s="6">
         <f t="shared" ca="1" si="14"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
     </row>
     <row r="99" spans="2:10" x14ac:dyDescent="0.25">
@@ -4809,7 +4839,7 @@
       </c>
       <c r="D99" s="5">
         <f t="shared" ca="1" si="17"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="E99" s="14">
         <f t="shared" ca="1" si="18"/>
@@ -4825,7 +4855,7 @@
       </c>
       <c r="H99" s="5">
         <f t="shared" ca="1" si="19"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="I99" s="5">
         <f t="shared" ca="1" si="13"/>
@@ -4833,7 +4863,7 @@
       </c>
       <c r="J99" s="6">
         <f t="shared" ca="1" si="14"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
     </row>
     <row r="100" spans="2:10" x14ac:dyDescent="0.25">
@@ -4847,7 +4877,7 @@
       </c>
       <c r="D100" s="5">
         <f t="shared" ca="1" si="17"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="E100" s="14">
         <f t="shared" ca="1" si="18"/>
@@ -4863,7 +4893,7 @@
       </c>
       <c r="H100" s="5">
         <f t="shared" ca="1" si="19"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="I100" s="5">
         <f t="shared" ca="1" si="13"/>
@@ -4871,7 +4901,7 @@
       </c>
       <c r="J100" s="6">
         <f t="shared" ca="1" si="14"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
     </row>
     <row r="101" spans="2:10" x14ac:dyDescent="0.25">
@@ -4885,7 +4915,7 @@
       </c>
       <c r="D101" s="5">
         <f t="shared" ca="1" si="17"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="E101" s="14">
         <f t="shared" ca="1" si="18"/>
@@ -4901,7 +4931,7 @@
       </c>
       <c r="H101" s="5">
         <f t="shared" ca="1" si="19"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="I101" s="5">
         <f t="shared" ca="1" si="13"/>
@@ -4909,7 +4939,7 @@
       </c>
       <c r="J101" s="6">
         <f t="shared" ca="1" si="14"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
     </row>
     <row r="102" spans="2:10" x14ac:dyDescent="0.25">
@@ -4923,7 +4953,7 @@
       </c>
       <c r="D102" s="5">
         <f t="shared" ca="1" si="17"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="E102" s="14">
         <f t="shared" ca="1" si="18"/>
@@ -4939,7 +4969,7 @@
       </c>
       <c r="H102" s="5">
         <f t="shared" ca="1" si="19"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="I102" s="5">
         <f t="shared" ca="1" si="13"/>
@@ -4947,7 +4977,7 @@
       </c>
       <c r="J102" s="6">
         <f t="shared" ca="1" si="14"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
     </row>
     <row r="103" spans="2:10" x14ac:dyDescent="0.25">
@@ -4961,7 +4991,7 @@
       </c>
       <c r="D103" s="5">
         <f t="shared" ca="1" si="17"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="E103" s="14">
         <f t="shared" ca="1" si="18"/>
@@ -4977,7 +5007,7 @@
       </c>
       <c r="H103" s="5">
         <f t="shared" ca="1" si="19"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="I103" s="5">
         <f t="shared" ca="1" si="13"/>
@@ -4985,7 +5015,7 @@
       </c>
       <c r="J103" s="6">
         <f t="shared" ca="1" si="14"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
     </row>
     <row r="104" spans="2:10" x14ac:dyDescent="0.25">
@@ -4999,7 +5029,7 @@
       </c>
       <c r="D104" s="5">
         <f t="shared" ca="1" si="17"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="E104" s="14">
         <f t="shared" ca="1" si="18"/>
@@ -5015,7 +5045,7 @@
       </c>
       <c r="H104" s="5">
         <f t="shared" ca="1" si="19"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="I104" s="5">
         <f t="shared" ca="1" si="13"/>
@@ -5023,7 +5053,7 @@
       </c>
       <c r="J104" s="6">
         <f t="shared" ca="1" si="14"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
     </row>
     <row r="105" spans="2:10" x14ac:dyDescent="0.25">
@@ -5037,7 +5067,7 @@
       </c>
       <c r="D105" s="5">
         <f t="shared" ca="1" si="17"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="E105" s="14">
         <f t="shared" ca="1" si="18"/>
@@ -5053,7 +5083,7 @@
       </c>
       <c r="H105" s="5">
         <f t="shared" ca="1" si="19"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="I105" s="5">
         <f t="shared" ca="1" si="13"/>
@@ -5061,7 +5091,7 @@
       </c>
       <c r="J105" s="6">
         <f t="shared" ref="J105:J109" ca="1" si="20">ROUND(H105+I105, 0)</f>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
     </row>
     <row r="106" spans="2:10" x14ac:dyDescent="0.25">
@@ -5075,7 +5105,7 @@
       </c>
       <c r="D106" s="5">
         <f t="shared" ca="1" si="17"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="E106" s="14">
         <f t="shared" ca="1" si="18"/>
@@ -5091,7 +5121,7 @@
       </c>
       <c r="H106" s="5">
         <f t="shared" ca="1" si="19"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="I106" s="5">
         <f t="shared" ca="1" si="13"/>
@@ -5099,7 +5129,7 @@
       </c>
       <c r="J106" s="6">
         <f t="shared" ca="1" si="20"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
     </row>
     <row r="107" spans="2:10" x14ac:dyDescent="0.25">
@@ -5113,7 +5143,7 @@
       </c>
       <c r="D107" s="5">
         <f t="shared" ca="1" si="17"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="E107" s="14">
         <f t="shared" ca="1" si="18"/>
@@ -5129,7 +5159,7 @@
       </c>
       <c r="H107" s="5">
         <f t="shared" ca="1" si="19"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="I107" s="5">
         <f t="shared" ca="1" si="13"/>
@@ -5137,7 +5167,7 @@
       </c>
       <c r="J107" s="6">
         <f t="shared" ca="1" si="20"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
     </row>
     <row r="108" spans="2:10" x14ac:dyDescent="0.25">
@@ -5151,7 +5181,7 @@
       </c>
       <c r="D108" s="5">
         <f t="shared" ca="1" si="17"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="E108" s="14">
         <f t="shared" ca="1" si="18"/>
@@ -5167,7 +5197,7 @@
       </c>
       <c r="H108" s="5">
         <f t="shared" ca="1" si="19"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="I108" s="5">
         <f t="shared" ca="1" si="13"/>
@@ -5175,7 +5205,7 @@
       </c>
       <c r="J108" s="6">
         <f t="shared" ca="1" si="20"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
     </row>
     <row r="109" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5189,7 +5219,7 @@
       </c>
       <c r="D109" s="9">
         <f t="shared" ca="1" si="17"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="E109" s="37">
         <f t="shared" ca="1" si="18"/>
@@ -5205,7 +5235,7 @@
       </c>
       <c r="H109" s="9">
         <f t="shared" ca="1" si="19"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
       <c r="I109" s="9">
         <f t="shared" ca="1" si="13"/>
@@ -5213,7 +5243,7 @@
       </c>
       <c r="J109" s="10">
         <f t="shared" ca="1" si="20"/>
-        <v>-52767</v>
+        <v>-4696792</v>
       </c>
     </row>
   </sheetData>
@@ -5283,7 +5313,7 @@
   <dimension ref="A1:N34"/>
   <sheetViews>
     <sheetView topLeftCell="A5" zoomScale="103" zoomScaleNormal="103" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5330,14 +5360,14 @@
     </row>
     <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="72" t="s">
+      <c r="B7" s="75" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="73"/>
-      <c r="E7" s="72" t="s">
+      <c r="C7" s="76"/>
+      <c r="E7" s="75" t="s">
         <v>52</v>
       </c>
-      <c r="F7" s="73"/>
+      <c r="F7" s="76"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
@@ -5433,7 +5463,7 @@
       </c>
       <c r="F14" s="48">
         <f>$C$24-SUM($C$25:$C$27)</f>
-        <v>1.0000000000000009E-2</v>
+        <v>2.0000000000000004E-2</v>
       </c>
       <c r="M14" s="45"/>
       <c r="N14" s="23"/>
@@ -5562,7 +5592,7 @@
         <v>39</v>
       </c>
       <c r="C27" s="57">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="M27" s="45"/>
       <c r="N27" s="51"/>
@@ -5623,7 +5653,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="pcH4kWynkl60A9Z/zPJEmKjiM0LI6Jv2Zl5G2E1wThfrT2fbOdGjXsB6LBbpzSALZ55wAdK37WamGnwrZyA0XA==" saltValue="s4BHSHNw3U7vqI0myjEszg==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="ngvSPMoSE8cL0ovX1bjYHNqTmyFqaKLI0uTIYGHxX8QsM8z71q7FRNUSPAgVfsLA8BA7n8xhcVYGT5g1ZFEthA==" saltValue="gVeLhGZfpfwrYXuCMRzQag==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0"/>
   <mergeCells count="2">
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="E7:F7"/>
@@ -5639,7 +5669,7 @@
   <dimension ref="A1:N45"/>
   <sheetViews>
     <sheetView zoomScale="94" zoomScaleNormal="49" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3:M8"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5659,11 +5689,11 @@
         <f>CONCATENATE("*Make sure total expense doesn't exceed monthly income of ", userMonthlyIncome )</f>
         <v>*Make sure total expense doesn't exceed monthly income of 50000</v>
       </c>
-      <c r="L1" s="74" t="s">
+      <c r="L1" s="77" t="s">
         <v>62</v>
       </c>
-      <c r="M1" s="74"/>
-      <c r="N1" s="74"/>
+      <c r="M1" s="77"/>
+      <c r="N1" s="77"/>
     </row>
     <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="L2" s="61"/>
@@ -5687,7 +5717,7 @@
       <c r="L3" s="61" t="s">
         <v>63</v>
       </c>
-      <c r="M3" s="13">
+      <c r="M3" s="74">
         <v>12000</v>
       </c>
       <c r="N3" s="63">
@@ -5696,7 +5726,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D4" s="65" t="s">
+      <c r="D4" s="11" t="s">
         <v>41</v>
       </c>
       <c r="E4" s="13">
@@ -5705,7 +5735,7 @@
       <c r="L4" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="M4" s="13">
+      <c r="M4" s="74">
         <v>6000</v>
       </c>
       <c r="N4" s="63">
@@ -5714,7 +5744,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D5" s="65" t="s">
+      <c r="D5" s="11" t="s">
         <v>42</v>
       </c>
       <c r="E5" s="13">
@@ -5723,7 +5753,7 @@
       <c r="L5" s="61" t="s">
         <v>65</v>
       </c>
-      <c r="M5" s="13">
+      <c r="M5" s="74">
         <v>3000</v>
       </c>
       <c r="N5" s="63">
@@ -5732,7 +5762,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D6" s="65" t="s">
+      <c r="D6" s="11" t="s">
         <v>43</v>
       </c>
       <c r="E6" s="13">
@@ -5741,7 +5771,7 @@
       <c r="L6" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="M6" s="13">
+      <c r="M6" s="74">
         <v>2000</v>
       </c>
       <c r="N6" s="63">
@@ -5750,7 +5780,7 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D7" s="65" t="s">
+      <c r="D7" s="11" t="s">
         <v>44</v>
       </c>
       <c r="E7" s="13">
@@ -5759,7 +5789,7 @@
       <c r="L7" s="61" t="s">
         <v>66</v>
       </c>
-      <c r="M7" s="13">
+      <c r="M7" s="74">
         <v>250</v>
       </c>
       <c r="N7" s="63">
@@ -5768,7 +5798,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D8" s="65" t="s">
+      <c r="D8" s="11" t="s">
         <v>45</v>
       </c>
       <c r="E8" s="13">
@@ -5777,7 +5807,7 @@
       <c r="L8" s="61" t="s">
         <v>67</v>
       </c>
-      <c r="M8" s="13">
+      <c r="M8" s="74">
         <v>100</v>
       </c>
       <c r="N8" s="63">
@@ -5786,7 +5816,7 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D9" s="65" t="s">
+      <c r="D9" s="11" t="s">
         <v>47</v>
       </c>
       <c r="E9" s="13">
@@ -5794,151 +5824,151 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D10" s="65"/>
+      <c r="D10" s="11"/>
       <c r="E10" s="13"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D11" s="65"/>
+      <c r="D11" s="11"/>
       <c r="E11" s="13"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D12" s="65"/>
+      <c r="D12" s="11"/>
       <c r="E12" s="13"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D13" s="65"/>
+      <c r="D13" s="11"/>
       <c r="E13" s="13"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D14" s="65"/>
+      <c r="D14" s="11"/>
       <c r="E14" s="13"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D15" s="65"/>
+      <c r="D15" s="11"/>
       <c r="E15" s="13"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D16" s="65"/>
+      <c r="D16" s="11"/>
       <c r="E16" s="13"/>
     </row>
     <row r="17" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D17" s="65"/>
+      <c r="D17" s="11"/>
       <c r="E17" s="13"/>
     </row>
     <row r="18" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D18" s="65"/>
+      <c r="D18" s="11"/>
       <c r="E18" s="13"/>
     </row>
     <row r="19" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D19" s="65"/>
+      <c r="D19" s="11"/>
       <c r="E19" s="13"/>
     </row>
     <row r="20" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D20" s="65"/>
+      <c r="D20" s="11"/>
       <c r="E20" s="13"/>
     </row>
     <row r="21" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D21" s="65"/>
+      <c r="D21" s="11"/>
       <c r="E21" s="13"/>
     </row>
     <row r="22" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D22" s="65"/>
+      <c r="D22" s="11"/>
       <c r="E22" s="13"/>
     </row>
     <row r="23" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D23" s="65"/>
+      <c r="D23" s="11"/>
       <c r="E23" s="13"/>
     </row>
     <row r="24" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D24" s="65"/>
+      <c r="D24" s="11"/>
       <c r="E24" s="13"/>
     </row>
     <row r="25" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D25" s="65"/>
+      <c r="D25" s="11"/>
       <c r="E25" s="13"/>
     </row>
     <row r="26" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D26" s="65"/>
+      <c r="D26" s="11"/>
       <c r="E26" s="13"/>
     </row>
     <row r="27" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D27" s="65"/>
+      <c r="D27" s="11"/>
       <c r="E27" s="13"/>
     </row>
     <row r="28" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D28" s="65"/>
+      <c r="D28" s="11"/>
       <c r="E28" s="13"/>
     </row>
     <row r="29" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D29" s="65"/>
+      <c r="D29" s="11"/>
       <c r="E29" s="13"/>
     </row>
     <row r="30" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D30" s="65"/>
+      <c r="D30" s="11"/>
       <c r="E30" s="13"/>
     </row>
     <row r="31" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D31" s="65"/>
+      <c r="D31" s="11"/>
       <c r="E31" s="13"/>
     </row>
     <row r="32" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D32" s="65"/>
+      <c r="D32" s="11"/>
       <c r="E32" s="13"/>
     </row>
     <row r="33" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D33" s="65"/>
+      <c r="D33" s="11"/>
       <c r="E33" s="13"/>
     </row>
     <row r="34" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D34" s="65"/>
+      <c r="D34" s="11"/>
       <c r="E34" s="13"/>
     </row>
     <row r="35" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D35" s="65"/>
+      <c r="D35" s="11"/>
       <c r="E35" s="13"/>
     </row>
     <row r="36" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D36" s="65"/>
+      <c r="D36" s="11"/>
       <c r="E36" s="13"/>
     </row>
     <row r="37" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D37" s="65"/>
+      <c r="D37" s="11"/>
       <c r="E37" s="13"/>
     </row>
     <row r="38" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D38" s="65"/>
+      <c r="D38" s="11"/>
       <c r="E38" s="13"/>
     </row>
     <row r="39" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D39" s="65"/>
+      <c r="D39" s="11"/>
       <c r="E39" s="13"/>
     </row>
     <row r="40" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D40" s="65"/>
+      <c r="D40" s="11"/>
       <c r="E40" s="13"/>
     </row>
     <row r="41" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D41" s="65"/>
+      <c r="D41" s="11"/>
       <c r="E41" s="13"/>
     </row>
     <row r="42" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D42" s="65"/>
+      <c r="D42" s="11"/>
       <c r="E42" s="13"/>
     </row>
     <row r="43" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D43" s="65"/>
+      <c r="D43" s="11"/>
       <c r="E43" s="13"/>
     </row>
     <row r="44" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D44" s="65"/>
+      <c r="D44" s="11"/>
       <c r="E44" s="13"/>
     </row>
     <row r="45" spans="4:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D45" s="66"/>
+      <c r="D45" s="68"/>
       <c r="E45" s="25"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="L3YzYyDQA1bLON4a9ZxbC4GyMpP02O/RSfhaGPlLj3F2zLqRkh9snzaQcnhxds7whHP3sQ2N8mPY0uVXTCanHw==" saltValue="aQJD5wNFNyAeu+YJCTMYoA==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="Qf+7FVYqiwdM2l7fmiUsRjU3fKuU3lgfSrEW4QcMfr7PfZvqImK9aI62flSH1w/W+zDioQyK1/huD+6NYMUD6g==" saltValue="0y6OmB+b1+nwE7LvqpcxQQ==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0"/>
   <mergeCells count="1">
     <mergeCell ref="L1:N1"/>
   </mergeCells>
@@ -5951,8 +5981,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:I106"/>
   <sheetViews>
-    <sheetView topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:E106"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5960,7 +5990,7 @@
     <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" customWidth="1"/>
     <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="66.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -5976,8 +6006,8 @@
         <v>50</v>
       </c>
       <c r="B3" s="63">
-        <f>SUMIF(F4:F106, "&gt;=0")</f>
-        <v>7250000</v>
+        <f>SUMIF($F$4:$F$106, "&gt;=0")</f>
+        <v>7050000</v>
       </c>
       <c r="D3" s="39" t="s">
         <v>10</v>
@@ -5994,8 +6024,8 @@
         <v>51</v>
       </c>
       <c r="B4" s="63">
-        <f>-SUMIF(F5:F107, "&lt;0")</f>
-        <v>10000000</v>
+        <f>-SUMIF($F$4:$F$106, "&lt;0")</f>
+        <v>11300000</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>7</v>
@@ -6131,16 +6161,12 @@
       <c r="F19" s="13"/>
     </row>
     <row r="20" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D20" s="11" t="s">
-        <v>54</v>
-      </c>
+      <c r="D20" s="11"/>
       <c r="E20" s="12"/>
       <c r="F20" s="13"/>
     </row>
     <row r="21" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D21" s="11" t="s">
-        <v>57</v>
-      </c>
+      <c r="D21" s="11"/>
       <c r="E21" s="12"/>
       <c r="F21" s="13"/>
     </row>
@@ -6540,56 +6566,73 @@
       <c r="F100" s="13"/>
     </row>
     <row r="101" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D101" s="11"/>
-      <c r="E101" s="12"/>
-      <c r="F101" s="13"/>
+      <c r="D101" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E101" s="12">
+        <v>35</v>
+      </c>
+      <c r="F101" s="13">
+        <v>-200000</v>
+      </c>
     </row>
     <row r="102" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D102" s="11"/>
-      <c r="E102" s="12"/>
-      <c r="F102" s="13"/>
+      <c r="D102" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E102" s="12">
+        <v>35</v>
+      </c>
+      <c r="F102" s="13">
+        <v>-100000</v>
+      </c>
     </row>
     <row r="103" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D103" s="11"/>
-      <c r="E103" s="12"/>
-      <c r="F103" s="13"/>
+      <c r="D103" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="E103" s="73">
+        <f>userRetirementAge</f>
+        <v>60</v>
+      </c>
+      <c r="F103" s="13">
+        <v>-1000000</v>
+      </c>
     </row>
     <row r="104" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D104" s="65" t="s">
         <v>61</v>
       </c>
-      <c r="E104" s="67">
+      <c r="E104" s="70">
         <f>userLifeExpectancyAge</f>
         <v>80</v>
       </c>
-      <c r="F104" s="13">
+      <c r="F104" s="25">
         <v>-10000000</v>
       </c>
     </row>
     <row r="105" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D105" s="68" t="s">
+      <c r="D105" s="66" t="s">
         <v>11</v>
       </c>
       <c r="E105" s="69">
         <f>userRetirementAge</f>
         <v>60</v>
       </c>
-      <c r="F105" s="13">
-        <v>200000</v>
-      </c>
+      <c r="F105" s="13"/>
     </row>
     <row r="106" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D106" s="70" t="s">
+      <c r="D106" s="67" t="s">
         <v>16</v>
       </c>
       <c r="E106" s="71">
         <f>userLifeExpectancyAge</f>
         <v>80</v>
       </c>
-      <c r="F106" s="13"/>
+      <c r="F106" s="72"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="rYcw/MWuTsC6WPH3FAB38a/Na4kyvi+L5UVWS5vni+Oq85uNTb4qhah4Iaa9VRPNcZs0/obx9wwaRITaYbqqag==" saltValue="WPNm2rQjXUy99qLtllRwqg==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="VzIdGTxkbZBJ4I/tIuYuO4GUJ3whJ44fWvpMNRnAOYzduF+1c+TuNznyA6BTvpfmB9bgjRrTtTJDCht4yQqt/Q==" saltValue="wzw5iCOk1kdvIe4aHdAFKg==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
@@ -6601,7 +6644,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6627,14 +6670,14 @@
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="72" t="s">
+      <c r="A5" s="75" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="73"/>
-      <c r="D5" s="72" t="s">
+      <c r="B5" s="76"/>
+      <c r="D5" s="75" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="73"/>
+      <c r="E5" s="76"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>

</xml_diff>